<commit_message>
update fig_temporal coverage and fig_archaeology
</commit_message>
<xml_diff>
--- a/fig_archaeology/arch_strat_consol.xlsx
+++ b/fig_archaeology/arch_strat_consol.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\git\road_paper\fig_archaeology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE726AE-E59B-4ACE-8627-B9438F815918}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED2BC08-6925-48F8-AFA3-3794A807F26B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2031" uniqueCount="659">
   <si>
     <t>Table archaeological_stratigraphy</t>
   </si>
@@ -1980,6 +1980,24 @@
   </si>
   <si>
     <t>simple search list 1 (n=40)</t>
+  </si>
+  <si>
+    <t>Other Early Stone Age</t>
+  </si>
+  <si>
+    <t>Other Late Stone Age</t>
+  </si>
+  <si>
+    <t>Other Middle Stone Age</t>
+  </si>
+  <si>
+    <t>Other Lower Paleolithic</t>
+  </si>
+  <si>
+    <t>Other Middle Paleolithic</t>
+  </si>
+  <si>
+    <t>Other Upper Paleolithic</t>
   </si>
 </sst>
 </file>
@@ -2122,7 +2140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2334,12 +2352,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -2517,20 +2529,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3284,8 +3294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B155" sqref="B155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3922,11 +3932,11 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>77</v>
+      <c r="A15" t="s">
+        <v>653</v>
       </c>
       <c r="B15" t="s">
-        <v>77</v>
+        <v>653</v>
       </c>
       <c r="C15" t="s">
         <v>77</v>
@@ -3972,7 +3982,7 @@
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B16" t="s">
@@ -4022,7 +4032,7 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="9" t="s">
         <v>640</v>
       </c>
       <c r="B17" t="s">
@@ -4078,7 +4088,7 @@
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B18" t="s">
@@ -4125,8 +4135,8 @@
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
-        <v>77</v>
+      <c r="A19" t="s">
+        <v>653</v>
       </c>
       <c r="B19" t="s">
         <v>97</v>
@@ -4172,11 +4182,11 @@
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>77</v>
+      <c r="A20" t="s">
+        <v>653</v>
       </c>
       <c r="B20" t="s">
-        <v>77</v>
+        <v>653</v>
       </c>
       <c r="C20" t="s">
         <v>77</v>
@@ -4222,11 +4232,11 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>77</v>
+      <c r="A21" t="s">
+        <v>653</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>653</v>
       </c>
       <c r="C21" t="s">
         <v>77</v>
@@ -4269,7 +4279,7 @@
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B22" t="s">
@@ -4428,7 +4438,7 @@
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B25" t="s">
@@ -4475,7 +4485,7 @@
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="9" t="s">
         <v>640</v>
       </c>
       <c r="B26" t="s">
@@ -4622,8 +4632,8 @@
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>77</v>
+      <c r="A29" t="s">
+        <v>653</v>
       </c>
       <c r="B29" t="s">
         <v>141</v>
@@ -4725,7 +4735,7 @@
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B31" t="s">
@@ -4775,7 +4785,7 @@
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B32" t="s">
@@ -4822,7 +4832,7 @@
       </c>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B33" t="s">
@@ -4875,8 +4885,8 @@
       </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>151</v>
+      <c r="A34" s="7" t="s">
+        <v>656</v>
       </c>
       <c r="B34" t="s">
         <v>171</v>
@@ -4984,8 +4994,8 @@
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
-        <v>151</v>
+      <c r="A36" s="7" t="s">
+        <v>656</v>
       </c>
       <c r="B36" t="s">
         <v>151</v>
@@ -5031,7 +5041,7 @@
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B37" t="s">
@@ -5075,8 +5085,8 @@
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A38" s="8" t="s">
-        <v>151</v>
+      <c r="A38" s="7" t="s">
+        <v>656</v>
       </c>
       <c r="B38" t="s">
         <v>151</v>
@@ -5128,7 +5138,7 @@
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B39" t="s">
@@ -5169,7 +5179,7 @@
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+      <c r="A40" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B40" t="s">
@@ -5213,7 +5223,7 @@
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="10" t="s">
+      <c r="A41" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B41" t="s">
@@ -5263,8 +5273,8 @@
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="8" t="s">
-        <v>151</v>
+      <c r="A42" s="7" t="s">
+        <v>656</v>
       </c>
       <c r="B42" t="s">
         <v>151</v>
@@ -5307,8 +5317,8 @@
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>151</v>
+      <c r="A43" s="7" t="s">
+        <v>656</v>
       </c>
       <c r="B43" t="s">
         <v>151</v>
@@ -5354,8 +5364,8 @@
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
-        <v>151</v>
+      <c r="A44" s="7" t="s">
+        <v>656</v>
       </c>
       <c r="B44" t="s">
         <v>151</v>
@@ -5392,8 +5402,8 @@
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
-        <v>151</v>
+      <c r="A45" s="7" t="s">
+        <v>656</v>
       </c>
       <c r="B45" t="s">
         <v>151</v>
@@ -5433,8 +5443,8 @@
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="8" t="s">
-        <v>151</v>
+      <c r="A46" s="7" t="s">
+        <v>656</v>
       </c>
       <c r="B46" t="s">
         <v>151</v>
@@ -5480,7 +5490,7 @@
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="8" t="s">
         <v>639</v>
       </c>
       <c r="B47" t="s">
@@ -5524,8 +5534,8 @@
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>151</v>
+      <c r="A48" s="7" t="s">
+        <v>656</v>
       </c>
       <c r="B48" t="s">
         <v>151</v>
@@ -5571,7 +5581,7 @@
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
+      <c r="A49" s="9" t="s">
         <v>640</v>
       </c>
       <c r="B49" t="s">
@@ -5609,7 +5619,7 @@
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="9" t="s">
         <v>640</v>
       </c>
       <c r="B50" t="s">
@@ -5653,8 +5663,8 @@
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A51" s="8" t="s">
-        <v>151</v>
+      <c r="A51" s="7" t="s">
+        <v>656</v>
       </c>
       <c r="B51" t="s">
         <v>151</v>
@@ -5771,8 +5781,8 @@
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>151</v>
+      <c r="A53" s="7" t="s">
+        <v>656</v>
       </c>
       <c r="B53" t="s">
         <v>260</v>
@@ -5918,11 +5928,11 @@
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
-        <v>272</v>
+      <c r="A56" t="s">
+        <v>654</v>
       </c>
       <c r="B56" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C56" t="s">
         <v>272</v>
@@ -5965,11 +5975,11 @@
       </c>
     </row>
     <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
-        <v>272</v>
+      <c r="A57" t="s">
+        <v>654</v>
       </c>
       <c r="B57" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C57" t="s">
         <v>272</v>
@@ -6015,11 +6025,11 @@
       </c>
     </row>
     <row r="58" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
-        <v>272</v>
+      <c r="A58" t="s">
+        <v>654</v>
       </c>
       <c r="B58" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C58" t="s">
         <v>272</v>
@@ -6062,11 +6072,11 @@
       </c>
     </row>
     <row r="59" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
-        <v>272</v>
+      <c r="A59" t="s">
+        <v>654</v>
       </c>
       <c r="B59" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C59" t="s">
         <v>272</v>
@@ -6103,11 +6113,11 @@
       </c>
     </row>
     <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
-        <v>272</v>
+      <c r="A60" t="s">
+        <v>654</v>
       </c>
       <c r="B60" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C60" t="s">
         <v>272</v>
@@ -6150,11 +6160,11 @@
       </c>
     </row>
     <row r="61" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
-        <v>272</v>
+      <c r="A61" t="s">
+        <v>654</v>
       </c>
       <c r="B61" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C61" t="s">
         <v>272</v>
@@ -6194,11 +6204,11 @@
       </c>
     </row>
     <row r="62" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A62" s="6" t="s">
-        <v>272</v>
+      <c r="A62" t="s">
+        <v>654</v>
       </c>
       <c r="B62" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C62" t="s">
         <v>272</v>
@@ -6238,11 +6248,11 @@
       </c>
     </row>
     <row r="63" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A63" s="6" t="s">
-        <v>272</v>
+      <c r="A63" t="s">
+        <v>654</v>
       </c>
       <c r="B63" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C63" t="s">
         <v>272</v>
@@ -6282,11 +6292,11 @@
       </c>
     </row>
     <row r="64" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A64" s="6" t="s">
-        <v>272</v>
+      <c r="A64" t="s">
+        <v>654</v>
       </c>
       <c r="B64" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C64" t="s">
         <v>272</v>
@@ -6379,11 +6389,11 @@
       </c>
     </row>
     <row r="66" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A66" s="6" t="s">
-        <v>272</v>
+      <c r="A66" t="s">
+        <v>654</v>
       </c>
       <c r="B66" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C66" t="s">
         <v>272</v>
@@ -6426,11 +6436,11 @@
       </c>
     </row>
     <row r="67" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
-        <v>272</v>
+      <c r="A67" t="s">
+        <v>654</v>
       </c>
       <c r="B67" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C67" t="s">
         <v>272</v>
@@ -6473,11 +6483,11 @@
       </c>
     </row>
     <row r="68" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
-        <v>272</v>
+      <c r="A68" t="s">
+        <v>654</v>
       </c>
       <c r="B68" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C68" t="s">
         <v>272</v>
@@ -6520,11 +6530,11 @@
       </c>
     </row>
     <row r="69" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A69" s="6" t="s">
-        <v>272</v>
+      <c r="A69" t="s">
+        <v>654</v>
       </c>
       <c r="B69" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C69" t="s">
         <v>272</v>
@@ -6561,11 +6571,11 @@
       </c>
     </row>
     <row r="70" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>272</v>
+      <c r="A70" t="s">
+        <v>654</v>
       </c>
       <c r="B70" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C70" t="s">
         <v>272</v>
@@ -6608,11 +6618,11 @@
       </c>
     </row>
     <row r="71" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
-        <v>272</v>
+      <c r="A71" t="s">
+        <v>654</v>
       </c>
       <c r="B71" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C71" t="s">
         <v>272</v>
@@ -6655,11 +6665,11 @@
       </c>
     </row>
     <row r="72" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A72" s="6" t="s">
-        <v>272</v>
+      <c r="A72" t="s">
+        <v>654</v>
       </c>
       <c r="B72" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C72" t="s">
         <v>272</v>
@@ -6702,11 +6712,11 @@
       </c>
     </row>
     <row r="73" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A73" s="6" t="s">
-        <v>272</v>
+      <c r="A73" t="s">
+        <v>654</v>
       </c>
       <c r="B73" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C73" t="s">
         <v>272</v>
@@ -6749,11 +6759,11 @@
       </c>
     </row>
     <row r="74" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
-        <v>272</v>
+      <c r="A74" t="s">
+        <v>654</v>
       </c>
       <c r="B74" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C74" t="s">
         <v>272</v>
@@ -6790,11 +6800,11 @@
       </c>
     </row>
     <row r="75" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
-        <v>272</v>
+      <c r="A75" t="s">
+        <v>654</v>
       </c>
       <c r="B75" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C75" t="s">
         <v>272</v>
@@ -6831,11 +6841,11 @@
       </c>
     </row>
     <row r="76" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>272</v>
+      <c r="A76" t="s">
+        <v>654</v>
       </c>
       <c r="B76" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C76" t="s">
         <v>272</v>
@@ -6872,11 +6882,11 @@
       </c>
     </row>
     <row r="77" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
-        <v>272</v>
+      <c r="A77" t="s">
+        <v>654</v>
       </c>
       <c r="B77" t="s">
-        <v>272</v>
+        <v>654</v>
       </c>
       <c r="C77" t="s">
         <v>272</v>
@@ -6981,11 +6991,11 @@
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A79" s="12" t="s">
-        <v>347</v>
+      <c r="A79" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="B79" t="s">
-        <v>347</v>
+        <v>657</v>
       </c>
       <c r="C79" t="s">
         <v>347</v>
@@ -7034,11 +7044,11 @@
       </c>
     </row>
     <row r="80" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A80" s="12" t="s">
-        <v>347</v>
+      <c r="A80" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="B80" t="s">
-        <v>347</v>
+        <v>657</v>
       </c>
       <c r="C80" t="s">
         <v>347</v>
@@ -7137,8 +7147,8 @@
       </c>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A82" s="12" t="s">
-        <v>347</v>
+      <c r="A82" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="B82" t="s">
         <v>366</v>
@@ -7190,7 +7200,7 @@
       </c>
     </row>
     <row r="83" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A83" s="7" t="s">
+      <c r="A83" s="6" t="s">
         <v>641</v>
       </c>
       <c r="B83" t="s">
@@ -7240,11 +7250,11 @@
       </c>
     </row>
     <row r="84" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A84" s="12" t="s">
-        <v>347</v>
+      <c r="A84" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="B84" t="s">
-        <v>347</v>
+        <v>657</v>
       </c>
       <c r="C84" t="s">
         <v>347</v>
@@ -7287,11 +7297,11 @@
       </c>
     </row>
     <row r="85" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A85" s="12" t="s">
-        <v>347</v>
+      <c r="A85" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="B85" t="s">
-        <v>347</v>
+        <v>657</v>
       </c>
       <c r="C85" t="s">
         <v>347</v>
@@ -7343,11 +7353,11 @@
       </c>
     </row>
     <row r="86" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A86" s="12" t="s">
-        <v>347</v>
+      <c r="A86" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="B86" t="s">
-        <v>347</v>
+        <v>657</v>
       </c>
       <c r="C86" t="s">
         <v>347</v>
@@ -7437,11 +7447,11 @@
       </c>
     </row>
     <row r="88" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A88" s="12" t="s">
-        <v>347</v>
+      <c r="A88" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="B88" t="s">
-        <v>347</v>
+        <v>657</v>
       </c>
       <c r="C88" t="s">
         <v>347</v>
@@ -7496,7 +7506,7 @@
       </c>
     </row>
     <row r="89" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="6" t="s">
         <v>641</v>
       </c>
       <c r="B89" t="s">
@@ -7546,7 +7556,7 @@
       </c>
     </row>
     <row r="90" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="6" t="s">
         <v>641</v>
       </c>
       <c r="B90" t="s">
@@ -7658,7 +7668,7 @@
       </c>
     </row>
     <row r="92" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A92" s="7" t="s">
+      <c r="A92" s="6" t="s">
         <v>641</v>
       </c>
       <c r="B92" t="s">
@@ -7708,11 +7718,11 @@
       </c>
     </row>
     <row r="93" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A93" s="12" t="s">
-        <v>347</v>
+      <c r="A93" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="B93" t="s">
-        <v>347</v>
+        <v>657</v>
       </c>
       <c r="C93" t="s">
         <v>347</v>
@@ -7764,11 +7774,11 @@
       </c>
     </row>
     <row r="94" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A94" s="12" t="s">
-        <v>347</v>
+      <c r="A94" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="B94" t="s">
-        <v>347</v>
+        <v>657</v>
       </c>
       <c r="C94" t="s">
         <v>347</v>
@@ -7808,11 +7818,11 @@
       </c>
     </row>
     <row r="95" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A95" s="12" t="s">
-        <v>347</v>
+      <c r="A95" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="B95" t="s">
-        <v>347</v>
+        <v>657</v>
       </c>
       <c r="C95" t="s">
         <v>347</v>
@@ -7852,11 +7862,11 @@
       </c>
     </row>
     <row r="96" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A96" s="12" t="s">
-        <v>347</v>
+      <c r="A96" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="B96" t="s">
-        <v>347</v>
+        <v>657</v>
       </c>
       <c r="C96" t="s">
         <v>347</v>
@@ -7899,11 +7909,11 @@
       </c>
     </row>
     <row r="97" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A97" s="12" t="s">
-        <v>347</v>
+      <c r="A97" s="10" t="s">
+        <v>657</v>
       </c>
       <c r="B97" t="s">
-        <v>347</v>
+        <v>657</v>
       </c>
       <c r="C97" t="s">
         <v>347</v>
@@ -7949,7 +7959,7 @@
       </c>
     </row>
     <row r="98" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A98" s="7" t="s">
+      <c r="A98" s="6" t="s">
         <v>641</v>
       </c>
       <c r="B98" t="s">
@@ -8002,7 +8012,7 @@
       </c>
     </row>
     <row r="99" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A99" s="7" t="s">
+      <c r="A99" s="6" t="s">
         <v>641</v>
       </c>
       <c r="B99" t="s">
@@ -8155,7 +8165,7 @@
       </c>
     </row>
     <row r="102" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A102" s="7" t="s">
+      <c r="A102" s="6" t="s">
         <v>641</v>
       </c>
       <c r="B102" t="s">
@@ -8264,11 +8274,11 @@
       </c>
     </row>
     <row r="104" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A104" s="10" t="s">
-        <v>454</v>
+      <c r="A104" t="s">
+        <v>655</v>
       </c>
       <c r="B104" t="s">
-        <v>454</v>
+        <v>655</v>
       </c>
       <c r="C104" t="s">
         <v>454</v>
@@ -8314,11 +8324,11 @@
       </c>
     </row>
     <row r="105" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A105" s="10" t="s">
-        <v>454</v>
+      <c r="A105" t="s">
+        <v>655</v>
       </c>
       <c r="B105" t="s">
-        <v>454</v>
+        <v>655</v>
       </c>
       <c r="C105" t="s">
         <v>454</v>
@@ -8361,11 +8371,11 @@
       </c>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A106" s="10" t="s">
-        <v>454</v>
+      <c r="A106" t="s">
+        <v>655</v>
       </c>
       <c r="B106" t="s">
-        <v>454</v>
+        <v>655</v>
       </c>
       <c r="C106" t="s">
         <v>454</v>
@@ -8399,8 +8409,8 @@
       </c>
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A107" s="10" t="s">
-        <v>454</v>
+      <c r="A107" t="s">
+        <v>655</v>
       </c>
       <c r="B107" t="s">
         <v>511</v>
@@ -8499,11 +8509,11 @@
       </c>
     </row>
     <row r="109" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A109" s="10" t="s">
-        <v>454</v>
+      <c r="A109" t="s">
+        <v>655</v>
       </c>
       <c r="B109" t="s">
-        <v>454</v>
+        <v>655</v>
       </c>
       <c r="C109" t="s">
         <v>454</v>
@@ -8593,8 +8603,8 @@
       </c>
     </row>
     <row r="111" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A111" s="10" t="s">
-        <v>454</v>
+      <c r="A111" t="s">
+        <v>655</v>
       </c>
       <c r="B111" t="s">
         <v>511</v>
@@ -8690,11 +8700,11 @@
       </c>
     </row>
     <row r="113" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A113" s="10" t="s">
-        <v>454</v>
+      <c r="A113" t="s">
+        <v>655</v>
       </c>
       <c r="B113" t="s">
-        <v>454</v>
+        <v>655</v>
       </c>
       <c r="C113" t="s">
         <v>454</v>
@@ -8737,11 +8747,11 @@
       </c>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A114" s="10" t="s">
-        <v>454</v>
+      <c r="A114" t="s">
+        <v>655</v>
       </c>
       <c r="B114" t="s">
-        <v>454</v>
+        <v>655</v>
       </c>
       <c r="C114" t="s">
         <v>454</v>
@@ -8781,11 +8791,11 @@
       </c>
     </row>
     <row r="115" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A115" s="10" t="s">
-        <v>454</v>
+      <c r="A115" t="s">
+        <v>655</v>
       </c>
       <c r="B115" t="s">
-        <v>454</v>
+        <v>655</v>
       </c>
       <c r="C115" t="s">
         <v>454</v>
@@ -8910,8 +8920,8 @@
       </c>
     </row>
     <row r="118" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A118" s="10" t="s">
-        <v>454</v>
+      <c r="A118" t="s">
+        <v>655</v>
       </c>
       <c r="B118" t="s">
         <v>511</v>
@@ -8963,11 +8973,11 @@
       </c>
     </row>
     <row r="119" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A119" s="10" t="s">
-        <v>454</v>
+      <c r="A119" t="s">
+        <v>655</v>
       </c>
       <c r="B119" t="s">
-        <v>454</v>
+        <v>655</v>
       </c>
       <c r="C119" t="s">
         <v>454</v>
@@ -9013,8 +9023,8 @@
       </c>
     </row>
     <row r="120" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A120" s="10" t="s">
-        <v>454</v>
+      <c r="A120" t="s">
+        <v>655</v>
       </c>
       <c r="B120" t="s">
         <v>511</v>
@@ -9119,11 +9129,11 @@
       </c>
     </row>
     <row r="122" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A122" s="10" t="s">
-        <v>454</v>
+      <c r="A122" t="s">
+        <v>655</v>
       </c>
       <c r="B122" t="s">
-        <v>454</v>
+        <v>655</v>
       </c>
       <c r="C122" t="s">
         <v>454</v>
@@ -9163,11 +9173,11 @@
       </c>
     </row>
     <row r="123" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A123" s="10" t="s">
-        <v>454</v>
+      <c r="A123" t="s">
+        <v>655</v>
       </c>
       <c r="B123" t="s">
-        <v>454</v>
+        <v>655</v>
       </c>
       <c r="C123" t="s">
         <v>454</v>
@@ -9207,11 +9217,11 @@
       </c>
     </row>
     <row r="124" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A124" s="10" t="s">
-        <v>454</v>
+      <c r="A124" t="s">
+        <v>655</v>
       </c>
       <c r="B124" t="s">
-        <v>454</v>
+        <v>655</v>
       </c>
       <c r="C124" t="s">
         <v>454</v>
@@ -9831,8 +9841,8 @@
       </c>
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A136" s="8" t="s">
-        <v>564</v>
+      <c r="A136" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B136" t="s">
         <v>563</v>
@@ -9881,11 +9891,11 @@
       </c>
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A137" s="8" t="s">
-        <v>564</v>
+      <c r="A137" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B137" t="s">
-        <v>564</v>
+        <v>658</v>
       </c>
       <c r="C137" t="s">
         <v>564</v>
@@ -9975,11 +9985,11 @@
       </c>
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A139" s="8" t="s">
-        <v>564</v>
+      <c r="A139" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B139" t="s">
-        <v>564</v>
+        <v>658</v>
       </c>
       <c r="C139" t="s">
         <v>564</v>
@@ -10025,8 +10035,8 @@
       </c>
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A140" s="8" t="s">
-        <v>564</v>
+      <c r="A140" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B140" t="s">
         <v>645</v>
@@ -10066,8 +10076,8 @@
       </c>
     </row>
     <row r="141" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A141" s="8" t="s">
-        <v>564</v>
+      <c r="A141" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B141" t="s">
         <v>645</v>
@@ -10204,8 +10214,8 @@
       </c>
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A144" s="8" t="s">
-        <v>564</v>
+      <c r="A144" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B144" t="s">
         <v>642</v>
@@ -10298,8 +10308,8 @@
       </c>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A146" s="8" t="s">
-        <v>564</v>
+      <c r="A146" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B146" t="s">
         <v>598</v>
@@ -10345,8 +10355,8 @@
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A147" s="8" t="s">
-        <v>564</v>
+      <c r="A147" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B147" t="s">
         <v>643</v>
@@ -10395,8 +10405,8 @@
       </c>
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A148" s="8" t="s">
-        <v>564</v>
+      <c r="A148" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B148" t="s">
         <v>608</v>
@@ -10533,11 +10543,11 @@
       </c>
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A151" s="8" t="s">
-        <v>564</v>
+      <c r="A151" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B151" t="s">
-        <v>564</v>
+        <v>658</v>
       </c>
       <c r="C151" t="s">
         <v>564</v>
@@ -10577,11 +10587,11 @@
       </c>
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A152" s="8" t="s">
-        <v>564</v>
+      <c r="A152" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B152" t="s">
-        <v>564</v>
+        <v>658</v>
       </c>
       <c r="C152" t="s">
         <v>564</v>
@@ -10618,11 +10628,11 @@
       </c>
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A153" s="8" t="s">
-        <v>564</v>
+      <c r="A153" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B153" t="s">
-        <v>564</v>
+        <v>658</v>
       </c>
       <c r="C153" t="s">
         <v>564</v>
@@ -10662,11 +10672,11 @@
       </c>
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A154" s="8" t="s">
-        <v>564</v>
+      <c r="A154" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B154" t="s">
-        <v>564</v>
+        <v>658</v>
       </c>
       <c r="C154" t="s">
         <v>564</v>
@@ -10709,11 +10719,11 @@
       </c>
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A155" s="8" t="s">
-        <v>564</v>
+      <c r="A155" s="7" t="s">
+        <v>658</v>
       </c>
       <c r="B155" t="s">
-        <v>564</v>
+        <v>658</v>
       </c>
       <c r="C155" t="s">
         <v>564</v>

</xml_diff>